<commit_message>
xlsx date object and ints
fixes
</commit_message>
<xml_diff>
--- a/Interpreter/Saves/data.xlsx
+++ b/Interpreter/Saves/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wew248\OneDrive\Course\2018\Semester 1\BCPR301 - Advanced Programming\Assignment\BCPR301---Assignment-1\BCPR301---Assignment-1\Saves\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\Course\2018\Semester 1\BCPR301 - Advanced Programming\Assignment\BCPR301---Assignment-1\BCPR301---Assignment-1\Interpreter\Saves\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_CF2E5A875C9582DD116FD05EEF161DEA26E075E0" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{D4DA4E59-6DE5-4F79-88AE-C1060E3C94A8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,43 +48,43 @@
     <t>Birthday</t>
   </si>
   <si>
-    <t>A23</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
     <t>normal</t>
   </si>
   <si>
-    <t>A24</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
     <t>Underweight</t>
   </si>
   <si>
-    <t>A25</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
     <t>Obesity</t>
   </si>
   <si>
-    <t>A26</t>
-  </si>
-  <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>A233</t>
+  </si>
+  <si>
+    <t>A244</t>
+  </si>
+  <si>
+    <t>A253</t>
+  </si>
+  <si>
+    <t>A262</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,15 +396,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -432,10 +434,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2">
         <v>22</v>
@@ -444,7 +446,7 @@
         <v>245</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <v>20</v>
@@ -455,10 +457,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -467,7 +469,7 @@
         <v>666</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>30</v>
@@ -478,10 +480,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>35</v>
@@ -490,7 +492,7 @@
         <v>456</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>55</v>
@@ -501,10 +503,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>24</v>
@@ -513,7 +515,7 @@
         <v>999</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>99</v>

</xml_diff>